<commit_message>
Switched formatting of bus reference voltages, now have complete admittance matrix including B factors and proper negation
</commit_message>
<xml_diff>
--- a/Data/PV_Bus_Reference_Voltages.xlsx
+++ b/Data/PV_Bus_Reference_Voltages.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JakeLaptop\Documents\GitHub\454_Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JakeLaptop\Documents\GitHub\454_Project\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{52C4F2FD-F699-4C4A-8BD2-8813DC6D5078}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C35ABAA-5A08-421C-90EF-3BD13A4A6CA4}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4410" xr2:uid="{A83EF6B4-0F6C-4472-B514-A589617B25B9}"/>
   </bookViews>
@@ -376,45 +376,51 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B65E26F3-C7E9-48F9-88E2-3AB6C7E66583}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection sqref="A1:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
       <c r="B1">
+        <v>1.05</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
         <v>2</v>
-      </c>
-      <c r="C1">
-        <v>3</v>
-      </c>
-      <c r="D1">
-        <v>10</v>
-      </c>
-      <c r="E1">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1.05</v>
       </c>
       <c r="B2">
         <v>1.0449999999999999</v>
       </c>
-      <c r="C2">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
         <v>1.01</v>
       </c>
-      <c r="D2">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>10</v>
+      </c>
+      <c r="B4">
         <v>1.05</v>
       </c>
-      <c r="E2">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>12</v>
+      </c>
+      <c r="B5">
         <v>1.05</v>
       </c>
     </row>

</xml_diff>